<commit_message>
feat: created class to store the columns needed for transactions creation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,259 +572,234 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>30116/2024 Project Jura - AMBEO Soundbar Soundfiles:</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+          <t>Datum</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bearbeiter</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tätigkeitsbeschreibung</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Dauer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Stunden-Satz</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Summe</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Datum
-Bearbeiter</t>
+          <t>19.09.2024</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tätigkeitsbeschreibung</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+          <t>Boytinck,Barbara (BEB)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>40551/2024 CHA-NI SE KG VAT reimbursement CHB Russia:Prüfung MSPA und LATA Russland; Telco mit C. Häußermann</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0,50</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>400,00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>200,00</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>25.09.2024 Dr. Schlaffge,</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>30116/2024 Project Jura: Durchsicht Mail Frau Kues und Prüfung</t>
-        </is>
-      </c>
+          <t>Gesamt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0,50</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>200,00</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Andrea (ACS)</t>
+          <t>Datum</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Behandlung Ambeo</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+          <t>Bearbeiter</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Tätigkeitsbeschreibung</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Dauer</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Stunden-Satz</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Summe</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>26.09.2024 Dr. Schlaffge,</t>
+          <t>25.09.2024</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>30116/2024 Project Jura - AMBEO Soundbar Soundfiles: Durchsicht</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+          <t>Dr. Schlaffge,Andrea (ACS)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>30116/2024 Project Jura: Durchsicht Mail Frau Kues und PrüfungBehandlung Ambeo</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0,25</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>500,00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>125,00</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Andrea (ACS)</t>
+          <t>26.09.2024</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>des LATA hinsichtl. Behandlung der AMBEO sound files</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+          <t>Dr. Schlaffge,Andrea (ACS)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>30116/2024 Project Jura - AMBEO Soundbar Soundfiles: Durchsichtdes LATA hinsichtl. Behandlung der AMBEO sound files</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0,50</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>500,00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>26.09.2024 Boytinck,</t>
+          <t>26.09.2024</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>30116/2024 Project Jura - AMBEO Soundbar Soundfiles: Prüfung</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+          <t>Boytinck,Barbara (BEB)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>30116/2024 Project Jura - AMBEO Soundbar Soundfiles: PrüfungLATA SE KG; Alignment mit A. Schlaffge; Telco mit C. Häußermannund Frau Kues</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1,25</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>400,00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>500,00</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Barbara (BEB)</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>LATA SE KG; Alignment mit A. Schlaffge; Telco mit C. Häußermann</t>
-        </is>
-      </c>
+          <t>Gesamt</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>und Frau Kues</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Gesamt</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Dauer</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Stunden-</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Summe</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Satz</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>0,25</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>500,00</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>125,00</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>0,50</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>500,00</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>250,00</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1,25</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>400,00</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>500,00</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>875,00</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>